<commit_message>
Model 1 and 2 working and ready for takeoff!!!!
</commit_message>
<xml_diff>
--- a/Data/PEM_efficiency_curve.xlsx
+++ b/Data/PEM_efficiency_curve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rolvur Reinert\Desktop\Thesis\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEFEAFCB-E264-472D-B64D-5BA94892DE93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1960318-04D9-407C-B2CA-B28A24C5344E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{9D2401FE-0EDF-7047-9218-8FB47D82F12E}"/>
+    <workbookView xWindow="350" yWindow="-10310" windowWidth="17280" windowHeight="8960" xr2:uid="{9D2401FE-0EDF-7047-9218-8FB47D82F12E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -264,25 +264,166 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>60</c:v>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -294,25 +435,166 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="54"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.3193049701884466E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>23.104209695952736</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.032093621114697</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.785662616162213</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.366897061730668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113.77774745299608</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136.02013496129942</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>158.09595198315293</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180.00706267695841</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201.75530348775646</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>223.34248366031795</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>244.77038574087737</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>266.04076606780194</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>287.15535525147862</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308.11585864369528</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>328.9239567967831</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>349.58130591278024</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>370.08953828286798</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>390.45026271732496</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>410.66506496623748</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>430.73550813119624</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>450.66313306820444</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>470.44945878201548</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>490.09598281211152</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>509.60418161053019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>528.97551091173773</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>548.21140609474503</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>567.31328253765537</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>586.28253596482523</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>605.12054278682263</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>623.82866043334957</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="31">
+                  <c:v>642.40822767930479</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>660.86056496414619</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>679.18697470471477</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>697.38874160167734</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>715.46713293973596</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>733.42339888175422</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>751.25877275694381</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>768.97447134324705</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>786.57169514405768</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>804.0516286594052</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="41">
+                  <c:v>821.41544065173696</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>838.66428440641982</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>855.79929798708417</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>872.82160448593072</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>889.73231226911184</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>906.53251521730544</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>923.22329296158534</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>939.80571111469987</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>956.2808214978586</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>972.64966236313182</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1130.7123854295805</c:v>
+                <c:pt idx="51">
+                  <c:v>988.91325861156065</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1005.0726220070715</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1021.1287513862932</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -592,60 +874,336 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$55</c:f>
+              <c:f>Sheet2!$A$2:$A$54</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>1.0000000000000001E-5</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>10</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>20</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>30</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="31">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>34</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>36</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>37</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>40</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="41">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>42</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>43</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>45</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>46</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>47</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>50</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>60</c:v>
+                <c:pt idx="51">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$55</c:f>
+              <c:f>Sheet2!$B$2:$B$54</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="54"/>
+                <c:ptCount val="53"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2.3193049701884466E-4</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>23.104209695952736</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.032093621114697</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.785662616162213</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>91.366897061730668</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>113.77774745299608</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>136.02013496129942</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>158.09595198315293</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>180.00706267695841</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>201.75530348775646</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>223.34248366031795</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="11">
+                  <c:v>244.77038574087737</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>266.04076606780194</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>287.15535525147862</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>308.11585864369528</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>328.9239567967831</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>349.58130591278024</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>370.08953828286798</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>390.45026271732496</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>410.66506496623748</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>430.73550813119624</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="21">
+                  <c:v>450.66313306820444</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>470.44945878201548</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>490.09598281211152</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>509.60418161053019</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>528.97551091173773</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>548.21140609474503</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>567.31328253765537</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>586.28253596482523</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>605.12054278682263</c:v>
+                </c:pt>
+                <c:pt idx="30">
                   <c:v>623.82866043334957</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="31">
+                  <c:v>642.40822767930479</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>660.86056496414619</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>679.18697470471477</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>697.38874160167734</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>715.46713293973596</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>733.42339888175422</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>751.25877275694381</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>768.97447134324705</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>786.57169514405768</c:v>
+                </c:pt>
+                <c:pt idx="40">
                   <c:v>804.0516286594052</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="41">
+                  <c:v>821.41544065173696</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>838.66428440641982</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>855.79929798708417</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>872.82160448593072</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>889.73231226911184</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>906.53251521730544</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>923.22329296158534</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>939.80571111469987</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>956.2808214978586</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>972.64966236313182</c:v>
                 </c:pt>
-                <c:pt idx="6">
-                  <c:v>1130.7123854295805</c:v>
+                <c:pt idx="51">
+                  <c:v>988.91325861156065</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1005.0726220070715</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1963,12 +2521,12 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
       <xdr:row>45</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>88900</xdr:colOff>
-      <xdr:row>63</xdr:row>
+      <xdr:row>60</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2006,8 +2564,8 @@
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2336,12 +2894,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{191039EE-5961-284E-A86E-0E1CC1829C94}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" zoomScale="75" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="23" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2355,20 +2914,20 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="B2">
         <f>($G$7*$G$3*$G$4*A2)/($G$5-$G$7*$G$4*$G$6*A2)</f>
-        <v>0</v>
+        <v>2.3193049701884466E-4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3" si="0">($G$7*$G$3*$G$4*A3)/($G$5-$G$7*$G$4*$G$6*A3)</f>
-        <v>223.34248366031795</v>
+        <f t="shared" ref="B3:B5" si="0">($G$7*$G$3*$G$4*A3)/($G$5-$G$7*$G$4*$G$6*A3)</f>
+        <v>23.104209695952736</v>
       </c>
       <c r="F3" t="s">
         <v>0</v>
@@ -2379,11 +2938,11 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <f t="shared" ref="B4:B24" si="1">($G$7*$G$3*$G$4*A4)/($G$5-$G$7*$G$4*$G$6*A4)</f>
-        <v>430.73550813119624</v>
+        <f t="shared" si="0"/>
+        <v>46.032093621114697</v>
       </c>
       <c r="F4" t="s">
         <v>3</v>
@@ -2394,198 +2953,480 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <f t="shared" si="0"/>
+        <v>68.785662616162213</v>
+      </c>
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="2">
+        <v>285830</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <f t="shared" ref="B6:B34" si="1">($G$7*$G$3*$G$4*A6)/($G$5-$G$7*$G$4*$G$6*A6)</f>
+        <v>91.366897061730668</v>
+      </c>
+      <c r="F6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G6" s="2">
+        <v>-1.51438605452536E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <f t="shared" si="1"/>
+        <v>113.77774745299608</v>
+      </c>
+      <c r="F7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2">
+        <v>3600000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>136.02013496129942</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>158.09595198315293</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>180.00706267695841</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>201.75530348775646</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>223.34248366031795</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>244.77038574087737</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>266.04076606780194</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>287.15535525147862</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>308.11585864369528</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>328.9239567967831</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>349.58130591278024</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>370.08953828286798</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>390.45026271732496</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>410.66506496623748</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>430.73550813119624</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>450.66313306820444</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <f t="shared" si="1"/>
+        <v>470.44945878201548</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <f t="shared" si="1"/>
+        <v>490.09598281211152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <f t="shared" si="1"/>
+        <v>509.60418161053019</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <f t="shared" si="1"/>
+        <v>528.97551091173773</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <f t="shared" si="1"/>
+        <v>548.21140609474503</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>567.31328253765537</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <f t="shared" si="1"/>
+        <v>586.28253596482523</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>605.12054278682263</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B5">
+      <c r="B32">
         <f t="shared" si="1"/>
         <v>623.82866043334957</v>
       </c>
-      <c r="F5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G5" s="2">
-        <v>285830</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>642.40822767930479</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
+        <v>32</v>
+      </c>
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>660.86056496414619</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <f t="shared" ref="B35:B54" si="2">($G$7*$G$3*$G$4*A35)/($G$5-$G$7*$G$4*$G$6*A35)</f>
+        <v>679.18697470471477</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="1">
+        <v>34</v>
+      </c>
+      <c r="B36">
+        <f t="shared" si="2"/>
+        <v>697.38874160167734</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="1">
+        <v>35</v>
+      </c>
+      <c r="B37">
+        <f t="shared" si="2"/>
+        <v>715.46713293973596</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="1">
+        <v>36</v>
+      </c>
+      <c r="B38">
+        <f t="shared" si="2"/>
+        <v>733.42339888175422</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="1">
+        <v>37</v>
+      </c>
+      <c r="B39">
+        <f t="shared" si="2"/>
+        <v>751.25877275694381</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="1">
+        <v>38</v>
+      </c>
+      <c r="B40">
+        <f t="shared" si="2"/>
+        <v>768.97447134324705</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="1">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <f t="shared" si="2"/>
+        <v>786.57169514405768</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B6">
-        <f t="shared" si="1"/>
+      <c r="B42">
+        <f t="shared" si="2"/>
         <v>804.0516286594052</v>
       </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" s="2">
-        <v>-1.51438605452536E-4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43">
+        <f t="shared" si="2"/>
+        <v>821.41544065173696</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44">
+        <f t="shared" si="2"/>
+        <v>838.66428440641982</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45">
+        <f t="shared" si="2"/>
+        <v>855.79929798708417</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46">
+        <f t="shared" si="2"/>
+        <v>872.82160448593072</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47">
+        <f t="shared" si="2"/>
+        <v>889.73231226911184</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <f t="shared" si="2"/>
+        <v>906.53251521730544</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49">
+        <f t="shared" si="2"/>
+        <v>923.22329296158534</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50">
+        <f t="shared" si="2"/>
+        <v>939.80571111469987</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <f t="shared" si="2"/>
+        <v>956.2808214978586</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B7">
-        <f t="shared" si="1"/>
+      <c r="B52">
+        <f t="shared" si="2"/>
         <v>972.64966236313182</v>
       </c>
-      <c r="F7" t="s">
-        <v>6</v>
-      </c>
-      <c r="G7" s="2">
-        <v>3600000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>60</v>
-      </c>
-      <c r="B8">
-        <f t="shared" si="1"/>
-        <v>1130.7123854295805</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <f t="shared" si="2"/>
+        <v>988.91325861156065</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <f t="shared" si="2"/>
+        <v>1005.0726220070715</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <f t="shared" ref="B55" si="3">($G$7*$G$3*$G$4*A55)/($G$5-$G$7*$G$4*$G$6*A55)</f>
+        <v>1021.1287513862932</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2603,8 +3444,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2BC684CE4692F40B415FEC87D586093" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d2dd4ab175ad0fcefda1366b6bfcffda">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a2f85246-06f9-4113-aded-c6f2279b8b6e" xmlns:ns3="c1503ef6-2b3d-436d-9aa2-08dd1e1e36bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c73b177c3784baaad4316a30c739546f" ns2:_="" ns3:_="">
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Notestaken xmlns="a2f85246-06f9-4113-aded-c6f2279b8b6e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a2f85246-06f9-4113-aded-c6f2279b8b6e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="c1503ef6-2b3d-436d-9aa2-08dd1e1e36bb" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100E2BC684CE4692F40B415FEC87D586093" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fc36c1e118a95775da8edfa7970c5c60">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a2f85246-06f9-4113-aded-c6f2279b8b6e" xmlns:ns3="c1503ef6-2b3d-436d-9aa2-08dd1e1e36bb" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bc71707077fa6f4a2e2b574616dc0bc0" ns2:_="" ns3:_="">
     <xsd:import namespace="a2f85246-06f9-4113-aded-c6f2279b8b6e"/>
     <xsd:import namespace="c1503ef6-2b3d-436d-9aa2-08dd1e1e36bb"/>
     <xsd:element name="properties">
@@ -2623,6 +3476,7 @@
                 <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -2683,6 +3537,11 @@
       </xsd:simpleType>
     </xsd:element>
     <xsd:element name="MediaServiceEventHashCode" ma:index="18" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="19" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
@@ -2802,18 +3661,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Notestaken xmlns="a2f85246-06f9-4113-aded-c6f2279b8b6e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a2f85246-06f9-4113-aded-c6f2279b8b6e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="c1503ef6-2b3d-436d-9aa2-08dd1e1e36bb" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F82A6CC-C4A5-43F2-B764-49A6C68C38F5}">
   <ds:schemaRefs>
@@ -2823,7 +3670,24 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BBB84CFF-00EC-476D-9E0D-CA094209FCAD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1B58244-24AA-4DCD-8269-8BF613E8610B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="c1503ef6-2b3d-436d-9aa2-08dd1e1e36bb"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="a2f85246-06f9-4113-aded-c6f2279b8b6e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5F7AFEC5-0659-4406-B8B4-66079B6D24B5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -2839,15 +3703,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F1B58244-24AA-4DCD-8269-8BF613E8610B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="a2f85246-06f9-4113-aded-c6f2279b8b6e"/>
-    <ds:schemaRef ds:uri="c1503ef6-2b3d-436d-9aa2-08dd1e1e36bb"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>